<commit_message>
Data change to Generate Report
</commit_message>
<xml_diff>
--- a/src/test/resources/data/IdExcel.xlsx
+++ b/src/test/resources/data/IdExcel.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsri3\WorkSpace\LMSRestAssured\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D27899-B1A3-4ABF-A7CE-29DA988D79E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321D8A4-F20E-45DD-98B4-9E1BBEC22A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ProgramID1</t>
   </si>
@@ -55,107 +55,28 @@
     <t>SubmissionId</t>
   </si>
   <si>
-    <t>U8106</t>
-  </si>
-  <si>
-    <t>U8107</t>
-  </si>
-  <si>
-    <t>U8108</t>
-  </si>
-  <si>
-    <t>9073</t>
-  </si>
-  <si>
-    <t>9074</t>
-  </si>
-  <si>
-    <t>June23-ninjalibaries-SDET11-150</t>
-  </si>
-  <si>
     <t>June23-ninjalibaries-SDET111-150</t>
   </si>
   <si>
-    <t>16593</t>
-  </si>
-  <si>
-    <t>16594</t>
-  </si>
-  <si>
-    <t>16620</t>
-  </si>
-  <si>
-    <t>16621</t>
-  </si>
-  <si>
-    <t>9535</t>
-  </si>
-  <si>
-    <t>9536</t>
-  </si>
-  <si>
-    <t>16862</t>
-  </si>
-  <si>
-    <t>16863</t>
-  </si>
-  <si>
-    <t>9686</t>
-  </si>
-  <si>
-    <t>9687</t>
-  </si>
-  <si>
-    <t>16898</t>
-  </si>
-  <si>
-    <t>June23-ninjalibaries-SDET111-111</t>
-  </si>
-  <si>
-    <t>16899</t>
-  </si>
-  <si>
-    <t>9703</t>
-  </si>
-  <si>
     <t>9704</t>
   </si>
   <si>
     <t>U11897</t>
   </si>
   <si>
-    <t>U11898</t>
-  </si>
-  <si>
     <t>U11899</t>
   </si>
   <si>
-    <t>5257</t>
-  </si>
-  <si>
-    <t>5258</t>
-  </si>
-  <si>
-    <t>16970</t>
-  </si>
-  <si>
     <t>U11981</t>
   </si>
   <si>
     <t>5308</t>
-  </si>
-  <si>
-    <t>5309</t>
-  </si>
-  <si>
-    <t>2196</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -465,34 +386,33 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="0"/>
-      <c r="B2" t="s" s="0">
-        <v>38</v>
+      <c r="B2">
+        <v>16970</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>32</v>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>9703</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>42</v>
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>2196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>